<commit_message>
Change to MEURyyyy currency format
Signed-off-by: Olexandr Balyk <olexandr.balyk@ucc.ie>
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_IND_CCS.xlsx
+++ b/SubRES_TMPL/SubRES_IND_CCS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C0FA27-E558-453B-BDC6-93F85B9BDF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2C26F-FE5F-475A-81FB-C2B9DDFAEB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="60" r:id="rId1"/>
@@ -530,9 +530,6 @@
     <t>MEUR/PJ</t>
   </si>
   <si>
-    <t>~FI_T: EUR10</t>
-  </si>
-  <si>
     <t>Exhange rate 2010</t>
   </si>
   <si>
@@ -609,6 +606,9 @@
   </si>
   <si>
     <t>Maurizio Gargiulo (E4SMA, maurizio.gargiulo@e4sma.com)</t>
+  </si>
+  <si>
+    <t>~FI_T: MEUR2010</t>
   </si>
 </sst>
 </file>
@@ -1658,25 +1658,25 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" style="22" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="22" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="22" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="22" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" style="22" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" style="22" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" style="22" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" style="22" customWidth="1"/>
     <col min="13" max="13" width="10" style="22" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="22" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="22" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="22"/>
+    <col min="14" max="14" width="11.3984375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" style="22" customWidth="1"/>
+    <col min="16" max="16384" width="8.86328125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1704,7 +1704,7 @@
       <c r="Y1" s="21"/>
       <c r="Z1" s="21"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -1732,7 +1732,7 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" s="20"/>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -1760,7 +1760,7 @@
       <c r="Y3" s="21"/>
       <c r="Z3" s="21"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -1788,7 +1788,7 @@
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -1816,7 +1816,7 @@
       <c r="Y5" s="21"/>
       <c r="Z5" s="21"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -1844,7 +1844,7 @@
       <c r="Y6" s="21"/>
       <c r="Z6" s="21"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -1872,7 +1872,7 @@
       <c r="Y7" s="21"/>
       <c r="Z7" s="21"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -1900,7 +1900,7 @@
       <c r="Y8" s="21"/>
       <c r="Z8" s="21"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -1928,7 +1928,7 @@
       <c r="Y9" s="21"/>
       <c r="Z9" s="21"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -1956,7 +1956,7 @@
       <c r="Y10" s="21"/>
       <c r="Z10" s="21"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -1984,7 +1984,7 @@
       <c r="Y11" s="21"/>
       <c r="Z11" s="21"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -2012,7 +2012,7 @@
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -2040,7 +2040,7 @@
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -2068,7 +2068,7 @@
       <c r="Y14" s="21"/>
       <c r="Z14" s="21"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
@@ -2096,9 +2096,9 @@
       <c r="Y15" s="21"/>
       <c r="Z15" s="21"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -2126,7 +2126,7 @@
       <c r="Y16" s="21"/>
       <c r="Z16" s="21"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -2154,7 +2154,7 @@
       <c r="Y17" s="21"/>
       <c r="Z17" s="21"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -2182,12 +2182,12 @@
       <c r="Y18" s="21"/>
       <c r="Z18" s="21"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="36"/>
       <c r="D19" s="36"/>
@@ -2214,12 +2214,12 @@
       <c r="Y19" s="21"/>
       <c r="Z19" s="21"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
@@ -2246,12 +2246,12 @@
       <c r="Y20" s="21"/>
       <c r="Z20" s="21"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
@@ -2278,7 +2278,7 @@
       <c r="Y21" s="21"/>
       <c r="Z21" s="21"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="28"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -2306,12 +2306,12 @@
       <c r="Y22" s="21"/>
       <c r="Z22" s="21"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="36"/>
       <c r="D23" s="36"/>
@@ -2338,10 +2338,10 @@
       <c r="Y23" s="21"/>
       <c r="Z23" s="21"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="28"/>
       <c r="B24" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="36"/>
       <c r="D24" s="36"/>
@@ -2368,10 +2368,10 @@
       <c r="Y24" s="21"/>
       <c r="Z24" s="21"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="28"/>
       <c r="B25" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
@@ -2398,12 +2398,12 @@
       <c r="Y25" s="21"/>
       <c r="Z25" s="21"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
@@ -2430,7 +2430,7 @@
       <c r="Y26" s="21"/>
       <c r="Z26" s="21"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="28"/>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -2458,7 +2458,7 @@
       <c r="Y27" s="21"/>
       <c r="Z27" s="21"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="28"/>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -2486,9 +2486,9 @@
       <c r="Y28" s="21"/>
       <c r="Z28" s="21"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="32">
         <v>1</v>
@@ -2518,12 +2518,12 @@
       <c r="Y29" s="21"/>
       <c r="Z29" s="21"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="38" t="s">
         <v>67</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>68</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
@@ -2550,12 +2550,12 @@
       <c r="Y30" s="21"/>
       <c r="Z30" s="21"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="36" t="s">
         <v>69</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>70</v>
       </c>
       <c r="C31" s="36"/>
       <c r="D31" s="36"/>
@@ -2582,10 +2582,10 @@
       <c r="Y31" s="21"/>
       <c r="Z31" s="21"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="34"/>
       <c r="B32" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -2612,7 +2612,7 @@
       <c r="Y32" s="21"/>
       <c r="Z32" s="21"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
@@ -2640,7 +2640,7 @@
       <c r="Y33" s="21"/>
       <c r="Z33" s="21"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
@@ -2668,7 +2668,7 @@
       <c r="Y34" s="21"/>
       <c r="Z34" s="21"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -2696,7 +2696,7 @@
       <c r="Y35" s="21"/>
       <c r="Z35" s="21"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -2724,7 +2724,7 @@
       <c r="Y36" s="21"/>
       <c r="Z36" s="21"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
@@ -2752,7 +2752,7 @@
       <c r="Y37" s="21"/>
       <c r="Z37" s="21"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
@@ -2780,7 +2780,7 @@
       <c r="Y38" s="21"/>
       <c r="Z38" s="21"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
@@ -2808,7 +2808,7 @@
       <c r="Y39" s="21"/>
       <c r="Z39" s="21"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -2836,7 +2836,7 @@
       <c r="Y40" s="21"/>
       <c r="Z40" s="21"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
@@ -2864,7 +2864,7 @@
       <c r="Y41" s="21"/>
       <c r="Z41" s="21"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
@@ -2892,7 +2892,7 @@
       <c r="Y42" s="21"/>
       <c r="Z42" s="21"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -2920,7 +2920,7 @@
       <c r="Y43" s="21"/>
       <c r="Z43" s="21"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -2948,7 +2948,7 @@
       <c r="Y44" s="21"/>
       <c r="Z44" s="21"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="21"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -2976,7 +2976,7 @@
       <c r="Y45" s="21"/>
       <c r="Z45" s="21"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -3004,7 +3004,7 @@
       <c r="Y46" s="21"/>
       <c r="Z46" s="21"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -3032,7 +3032,7 @@
       <c r="Y47" s="21"/>
       <c r="Z47" s="21"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="21"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -3060,7 +3060,7 @@
       <c r="Y48" s="21"/>
       <c r="Z48" s="21"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="21"/>
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
@@ -3088,7 +3088,7 @@
       <c r="Y49" s="21"/>
       <c r="Z49" s="21"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="21"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -3116,7 +3116,7 @@
       <c r="Y50" s="21"/>
       <c r="Z50" s="21"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -3144,7 +3144,7 @@
       <c r="Y51" s="21"/>
       <c r="Z51" s="21"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="21"/>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -3172,7 +3172,7 @@
       <c r="Y52" s="21"/>
       <c r="Z52" s="21"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -3200,7 +3200,7 @@
       <c r="Y53" s="21"/>
       <c r="Z53" s="21"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="21"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -3228,7 +3228,7 @@
       <c r="Y54" s="21"/>
       <c r="Z54" s="21"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -3256,7 +3256,7 @@
       <c r="Y55" s="21"/>
       <c r="Z55" s="21"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="21"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -3284,7 +3284,7 @@
       <c r="Y56" s="21"/>
       <c r="Z56" s="21"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="21"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -3312,7 +3312,7 @@
       <c r="Y57" s="21"/>
       <c r="Z57" s="21"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="21"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -3340,7 +3340,7 @@
       <c r="Y58" s="21"/>
       <c r="Z58" s="21"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="21"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
@@ -3368,7 +3368,7 @@
       <c r="Y59" s="21"/>
       <c r="Z59" s="21"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -3396,7 +3396,7 @@
       <c r="Y60" s="21"/>
       <c r="Z60" s="21"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="21"/>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
@@ -3424,7 +3424,7 @@
       <c r="Y61" s="21"/>
       <c r="Z61" s="21"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="21"/>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
@@ -3452,7 +3452,7 @@
       <c r="Y62" s="21"/>
       <c r="Z62" s="21"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -3480,7 +3480,7 @@
       <c r="Y63" s="21"/>
       <c r="Z63" s="21"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="21"/>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -3508,7 +3508,7 @@
       <c r="Y64" s="21"/>
       <c r="Z64" s="21"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
@@ -3536,7 +3536,7 @@
       <c r="Y65" s="21"/>
       <c r="Z65" s="21"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" s="21"/>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
@@ -3564,7 +3564,7 @@
       <c r="Y66" s="21"/>
       <c r="Z66" s="21"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" s="21"/>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
@@ -3592,7 +3592,7 @@
       <c r="Y67" s="21"/>
       <c r="Z67" s="21"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" s="21"/>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
@@ -3620,7 +3620,7 @@
       <c r="Y68" s="21"/>
       <c r="Z68" s="21"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A69" s="21"/>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
@@ -3648,7 +3648,7 @@
       <c r="Y69" s="21"/>
       <c r="Z69" s="21"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
@@ -3676,7 +3676,7 @@
       <c r="Y70" s="21"/>
       <c r="Z70" s="21"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" s="21"/>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
@@ -3704,7 +3704,7 @@
       <c r="Y71" s="21"/>
       <c r="Z71" s="21"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="21"/>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
@@ -3732,7 +3732,7 @@
       <c r="Y72" s="21"/>
       <c r="Z72" s="21"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -3760,7 +3760,7 @@
       <c r="Y73" s="21"/>
       <c r="Z73" s="21"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -3788,7 +3788,7 @@
       <c r="Y74" s="21"/>
       <c r="Z74" s="21"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
@@ -3816,7 +3816,7 @@
       <c r="Y75" s="21"/>
       <c r="Z75" s="21"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" s="21"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
@@ -3844,7 +3844,7 @@
       <c r="Y76" s="21"/>
       <c r="Z76" s="21"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -3872,7 +3872,7 @@
       <c r="Y77" s="21"/>
       <c r="Z77" s="21"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" s="21"/>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
@@ -3900,7 +3900,7 @@
       <c r="Y78" s="21"/>
       <c r="Z78" s="21"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
@@ -3928,7 +3928,7 @@
       <c r="Y79" s="21"/>
       <c r="Z79" s="21"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" s="21"/>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
@@ -3956,7 +3956,7 @@
       <c r="Y80" s="21"/>
       <c r="Z80" s="21"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" s="21"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
@@ -3984,7 +3984,7 @@
       <c r="Y81" s="21"/>
       <c r="Z81" s="21"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
@@ -4012,7 +4012,7 @@
       <c r="Y82" s="21"/>
       <c r="Z82" s="21"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="21"/>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
@@ -4040,7 +4040,7 @@
       <c r="Y83" s="21"/>
       <c r="Z83" s="21"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
@@ -4068,7 +4068,7 @@
       <c r="Y84" s="21"/>
       <c r="Z84" s="21"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="21"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
@@ -4096,7 +4096,7 @@
       <c r="Y85" s="21"/>
       <c r="Z85" s="21"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
@@ -4124,7 +4124,7 @@
       <c r="Y86" s="21"/>
       <c r="Z86" s="21"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" s="21"/>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
@@ -4152,7 +4152,7 @@
       <c r="Y87" s="21"/>
       <c r="Z87" s="21"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
@@ -4180,7 +4180,7 @@
       <c r="Y88" s="21"/>
       <c r="Z88" s="21"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A89" s="21"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -4208,7 +4208,7 @@
       <c r="Y89" s="21"/>
       <c r="Z89" s="21"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -4236,7 +4236,7 @@
       <c r="Y90" s="21"/>
       <c r="Z90" s="21"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A91" s="21"/>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
@@ -4264,7 +4264,7 @@
       <c r="Y91" s="21"/>
       <c r="Z91" s="21"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
@@ -4292,7 +4292,7 @@
       <c r="Y92" s="21"/>
       <c r="Z92" s="21"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A93" s="21"/>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
@@ -4320,7 +4320,7 @@
       <c r="Y93" s="21"/>
       <c r="Z93" s="21"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
@@ -4348,7 +4348,7 @@
       <c r="Y94" s="21"/>
       <c r="Z94" s="21"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A95" s="21"/>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
@@ -4376,7 +4376,7 @@
       <c r="Y95" s="21"/>
       <c r="Z95" s="21"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A96" s="21"/>
       <c r="B96" s="21"/>
       <c r="C96" s="21"/>
@@ -4404,7 +4404,7 @@
       <c r="Y96" s="21"/>
       <c r="Z96" s="21"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A97" s="21"/>
       <c r="B97" s="21"/>
       <c r="C97" s="21"/>
@@ -4432,7 +4432,7 @@
       <c r="Y97" s="21"/>
       <c r="Z97" s="21"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A98" s="21"/>
       <c r="B98" s="21"/>
       <c r="C98" s="21"/>
@@ -4460,7 +4460,7 @@
       <c r="Y98" s="21"/>
       <c r="Z98" s="21"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A99" s="21"/>
       <c r="B99" s="21"/>
       <c r="C99" s="21"/>
@@ -4515,37 +4515,37 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:T23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.73046875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" style="3" customWidth="1"/>
     <col min="9" max="9" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="67.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="9.42578125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="3"/>
+    <col min="10" max="10" width="14.86328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.265625" style="3" customWidth="1"/>
+    <col min="12" max="13" width="9.1328125" style="3"/>
+    <col min="14" max="14" width="15.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="67.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.3984375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.3984375" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -4565,7 +4565,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4582,13 +4582,13 @@
         <v>22</v>
       </c>
       <c r="F4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>23</v>
@@ -4597,7 +4597,7 @@
         <v>24</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>6</v>
@@ -4624,9 +4624,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>10</v>
@@ -4644,7 +4644,7 @@
         <v>28</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15" t="s">
@@ -4681,7 +4681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -4712,7 +4712,7 @@
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="str">
         <f>N7</f>
         <v>I-DMD-ONM-N1</v>
@@ -4768,7 +4768,7 @@
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C13" s="3" t="s">
         <v>40</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C14" s="3" t="s">
         <v>41</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
@@ -4875,20 +4875,20 @@
       </c>
       <c r="K16" s="17"/>
     </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="9:11" x14ac:dyDescent="0.35">
       <c r="I22" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I23" s="11" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I23" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="J23" s="12">
         <v>0.86080000000000001</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>